<commit_message>
preprocessing and function exploration
</commit_message>
<xml_diff>
--- a/Docs/var_list.xlsx
+++ b/Docs/var_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="283">
   <si>
     <t xml:space="preserve">code</t>
   </si>
@@ -28,16 +28,28 @@
     <t xml:space="preserve">label</t>
   </si>
   <si>
-    <t xml:space="preserve">expl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categoria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sost</t>
+    <t xml:space="preserve">explanation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new_label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA_strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked_var</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked_var_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">replace_NA_with</t>
   </si>
   <si>
     <t xml:space="preserve">PROFAM</t>
@@ -61,7 +73,7 @@
     <t xml:space="preserve">numero componenti nucleo familiare</t>
   </si>
   <si>
-    <t xml:space="preserve">demografiche</t>
+    <t xml:space="preserve">demographics</t>
   </si>
   <si>
     <t xml:space="preserve">ETAMi</t>
@@ -82,6 +94,9 @@
     <t xml:space="preserve">stato civile</t>
   </si>
   <si>
+    <t xml:space="preserve">9=not available</t>
+  </si>
+  <si>
     <t xml:space="preserve">AMATR</t>
   </si>
   <si>
@@ -94,7 +109,7 @@
     <t xml:space="preserve">titolo studio</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
+    <t xml:space="preserve">99=not available</t>
   </si>
   <si>
     <t xml:space="preserve">CONDMi</t>
@@ -103,7 +118,7 @@
     <t xml:space="preserve">condizione professionale</t>
   </si>
   <si>
-    <t xml:space="preserve">lavoro</t>
+    <t xml:space="preserve">work_life</t>
   </si>
   <si>
     <t xml:space="preserve">LAVPAS  </t>
@@ -112,12 +127,24 @@
     <t xml:space="preserve">ha lavorato in passato</t>
   </si>
   <si>
+    <t xml:space="preserve">Nas are for CONDMi=1 (occupato). Substitute these Nas with 3=now working, unknown if worked in the past</t>
+  </si>
+  <si>
     <t xml:space="preserve">POSIZMi</t>
   </si>
   <si>
     <t xml:space="preserve">posizione nella professione     </t>
   </si>
   <si>
+    <t xml:space="preserve">Nas are for CONDMi=3 (inattivo) and 2(looking for job). Substitute these Nas with 5=not in any working position (inactive) and 6= not in any working position (looking for)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3, 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5, 6</t>
+  </si>
+  <si>
     <t xml:space="preserve">CITTMi</t>
   </si>
   <si>
@@ -130,7 +157,13 @@
     <t xml:space="preserve">lezioni private informatica</t>
   </si>
   <si>
-    <t xml:space="preserve">istruzione</t>
+    <t xml:space="preserve">free_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aggregare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEMLIB_CLASSES</t>
   </si>
   <si>
     <t xml:space="preserve">LING</t>
@@ -151,7 +184,10 @@
     <t xml:space="preserve">att. fisica lavoro domestico</t>
   </si>
   <si>
-    <t xml:space="preserve">attività fisica</t>
+    <t xml:space="preserve">physical_act</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHYS_ACT_daily</t>
   </si>
   <si>
     <t xml:space="preserve">TLAV</t>
@@ -160,19 +196,25 @@
     <t xml:space="preserve">att. fisica al lavoro</t>
   </si>
   <si>
+    <t xml:space="preserve">Nas are for CONDMi=1 (occupato). Substitute these Nas with 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">NPROSOM</t>
   </si>
   <si>
     <t xml:space="preserve">quante volte al PS ultimi 3 mesi</t>
   </si>
   <si>
-    <t xml:space="preserve">salute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aggregare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASSIST_SANITARIA</t>
+    <t xml:space="preserve">physical_health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS_aggr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nas are for PROSOC=1 (NO). Substitute these Nas with 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROSOC</t>
   </si>
   <si>
     <t xml:space="preserve">NGUMEDM</t>
@@ -181,16 +223,25 @@
     <t xml:space="preserve">quante volte in guardia medica ultimi 3 mesi</t>
   </si>
   <si>
+    <t xml:space="preserve">NAs are for GUMED=3 (no). Substitute these Nas with 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUMED</t>
+  </si>
+  <si>
     <t xml:space="preserve">NASSDOM</t>
   </si>
   <si>
     <t xml:space="preserve">quante volte ricorso ad assistenza domiciliare ultimi 3 mesi</t>
   </si>
   <si>
-    <t xml:space="preserve"> NNRICAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quante volte ricoverato ultimi 3 mesi</t>
+    <t xml:space="preserve">HOSP_STAY_aggr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nas are for ASSDO=5 (no), substitute these Nas with 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASSDO</t>
   </si>
   <si>
     <t xml:space="preserve">GGRICAM</t>
@@ -199,22 +250,34 @@
     <t xml:space="preserve">quante notti ricoverato ultimi 3 mesi</t>
   </si>
   <si>
+    <t xml:space="preserve">Nas are for RICOV=1(no). Substitute these values with 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RICOV</t>
+  </si>
+  <si>
     <t xml:space="preserve">VSPESA</t>
   </si>
   <si>
     <t xml:space="preserve">spesa per ultima visita specialistica ultimi 12 mesi   </t>
   </si>
   <si>
-    <t xml:space="preserve">NINCDOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incidente domestico subito negli ultimi 12 mesi: quante volte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MNINCDM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incidente domestico subito negli ultimi 3 mesi: quante volte   </t>
+    <t xml:space="preserve">Nas are for VISMED12=1 (no)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VISMED12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATTFIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le capita di svolgere nel tempo libero qualche attività fisica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nas are for SPOCON=1 (no). Substitute these values with 1=no, never</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPOCON</t>
   </si>
   <si>
     <t xml:space="preserve">FREQSPO</t>
@@ -229,13 +292,16 @@
     <t xml:space="preserve">Ore di attivit sportiva praticate nell'ultima settimana  </t>
   </si>
   <si>
+    <t xml:space="preserve">Nas are for SPOCON=1 (no). Substitute these values with 8=never this year</t>
+  </si>
+  <si>
     <t xml:space="preserve">AMICI</t>
   </si>
   <si>
     <t xml:space="preserve">frequenza appuntamenti con amici</t>
   </si>
   <si>
-    <t xml:space="preserve">vita sociale – non strutturata</t>
+    <t xml:space="preserve">social_life</t>
   </si>
   <si>
     <t xml:space="preserve">PARENT</t>
@@ -262,7 +328,7 @@
     <t xml:space="preserve">freq consumo pane pasta</t>
   </si>
   <si>
-    <t xml:space="preserve">alimentazione</t>
+    <t xml:space="preserve">eating_habits</t>
   </si>
   <si>
     <t xml:space="preserve">SALUMI</t>
@@ -304,6 +370,9 @@
     <t xml:space="preserve">frequenza consumo latte</t>
   </si>
   <si>
+    <t xml:space="preserve">LATTICINI_aggr</t>
+  </si>
+  <si>
     <t xml:space="preserve">FORM</t>
   </si>
   <si>
@@ -367,7 +436,7 @@
     <t xml:space="preserve">quantità abituale birra</t>
   </si>
   <si>
-    <t xml:space="preserve">consumo alcolici</t>
+    <t xml:space="preserve">alcohol_habits</t>
   </si>
   <si>
     <t xml:space="preserve">ALCOL_abituale_aggr</t>
@@ -388,12 +457,21 @@
     <t xml:space="preserve">ALCOL_unità_giorno_aggr</t>
   </si>
   <si>
+    <t xml:space="preserve">Nas are for BIRRA=4,5,6. Substitute these values with 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,5,6</t>
+  </si>
+  <si>
     <t xml:space="preserve">BICVINOM  </t>
   </si>
   <si>
     <t xml:space="preserve">quanti bicchieri vino giorno </t>
   </si>
   <si>
+    <t xml:space="preserve">Nas are for VINO=4,5,6. Substitute these values with 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">BFPAS</t>
   </si>
   <si>
@@ -406,6 +484,12 @@
     <t xml:space="preserve">quanti bicchieri di alcolici fuori dai pasti in una settimana </t>
   </si>
   <si>
+    <t xml:space="preserve">Nas are for BFPAS=3,4. Substitute these values with 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3, 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">ALCOL</t>
   </si>
   <si>
@@ -424,25 +508,25 @@
     <t xml:space="preserve">quantità abituale liquori</t>
   </si>
   <si>
-    <t xml:space="preserve">BICALTROM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n. bicchieri al giorno di aperitivi alcolici, amari o superalcolici</t>
-  </si>
-  <si>
     <t xml:space="preserve">NBICALCM</t>
   </si>
   <si>
     <t xml:space="preserve">Consumo di almeno 6 bicchieri di bevande alcoliche in un'unica occasione negli ultimi 12 mesi: numero di volte</t>
   </si>
   <si>
+    <t xml:space="preserve">Nas are for BICALC=1 (no). Substitute these values with 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BICALC</t>
+  </si>
+  <si>
     <t xml:space="preserve">FUMO</t>
   </si>
   <si>
     <t xml:space="preserve">attualmente fuma</t>
   </si>
   <si>
-    <t xml:space="preserve">fumo</t>
+    <t xml:space="preserve">smoking_habits</t>
   </si>
   <si>
     <t xml:space="preserve">FRFUMO  </t>
@@ -451,18 +535,30 @@
     <t xml:space="preserve">freq fumo</t>
   </si>
   <si>
+    <t xml:space="preserve">Nas are for FUMO=2,3 (not smoking at the present moment). Substitute these values with 3=never</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2, 3</t>
+  </si>
+  <si>
     <t xml:space="preserve"> NSIGARM</t>
   </si>
   <si>
     <t xml:space="preserve">n. sigarette/giorno</t>
   </si>
   <si>
+    <t xml:space="preserve">Nas are for FUMO=2,3 (not smoking at the present moment). Substitute these values with 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">SALUTE</t>
   </si>
   <si>
     <t xml:space="preserve">come va salute in generale</t>
   </si>
   <si>
+    <t xml:space="preserve">health_opinion</t>
+  </si>
+  <si>
     <t xml:space="preserve">CRONI</t>
   </si>
   <si>
@@ -481,7 +577,7 @@
     <t xml:space="preserve">quanto tempo nelle ultime 4 settimane sentito sereno</t>
   </si>
   <si>
-    <t xml:space="preserve">benessere psicologico</t>
+    <t xml:space="preserve">psychological_wellbeing</t>
   </si>
   <si>
     <t xml:space="preserve">                                                                             </t>
@@ -520,42 +616,42 @@
     <t xml:space="preserve">HHRAD</t>
   </si>
   <si>
-    <t xml:space="preserve">ore ascolto radio/giorno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tempo libero</t>
+    <t xml:space="preserve">quante ore ascolta radio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nas are for RADIO=1 (no). Substitute these values with 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RADIO</t>
   </si>
   <si>
     <t xml:space="preserve">HHTEL</t>
   </si>
   <si>
-    <t xml:space="preserve">ore tele/giorno</t>
+    <t xml:space="preserve">quante ore guarda tv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nas are for TELE=1 (no). Substitute these values with 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TELE</t>
   </si>
   <si>
     <t xml:space="preserve">FREQSERIE</t>
   </si>
   <si>
-    <t xml:space="preserve">freq serie tv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUMBIBM  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">quante volte biblio ultimi 12 mesi </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tempo libero – attività culturali</t>
+    <t xml:space="preserve">frequenza serie tv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEATRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freq teatro ultimi 12 mesi</t>
   </si>
   <si>
     <t xml:space="preserve">ATT_CULT_aggr</t>
   </si>
   <si>
-    <t xml:space="preserve">TEATRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">freq teatro ultimi 12 mesi</t>
-  </si>
-  <si>
     <t xml:space="preserve">CINE  </t>
   </si>
   <si>
@@ -598,27 +694,12 @@
     <t xml:space="preserve">freq visite siti monumentali ultimi 12 mesi</t>
   </si>
   <si>
-    <t xml:space="preserve">FREQPC12  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frequenza uso pc negli ultimi 12 mesi </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FREQIN12  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frequenza uso internet negli ultimi 12 mesi</t>
-  </si>
-  <si>
     <t xml:space="preserve">LQUOT</t>
   </si>
   <si>
     <t xml:space="preserve">legge quotidiani almeno 1 volta la settimana</t>
   </si>
   <si>
-    <t xml:space="preserve">tempo libero – lettura quotidiani</t>
-  </si>
-  <si>
     <t xml:space="preserve">LETTURA_QUOT_aggr</t>
   </si>
   <si>
@@ -634,12 +715,15 @@
     <t xml:space="preserve">n libri letti ultimi 12 mesi</t>
   </si>
   <si>
-    <t xml:space="preserve">tempo libero – lettura libri</t>
-  </si>
-  <si>
     <t xml:space="preserve">LETTURA_LIBRI_aggr</t>
   </si>
   <si>
+    <t xml:space="preserve">Nas are for LIBRI=1 (no). Substitute these values with 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIBRI</t>
+  </si>
+  <si>
     <t xml:space="preserve">NLIBRI_CARM</t>
   </si>
   <si>
@@ -652,19 +736,13 @@
     <t xml:space="preserve">n ebook ultimi 12 mesi</t>
   </si>
   <si>
-    <t xml:space="preserve">NLAUDIOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n audiolibri ultimi 12 mesi</t>
-  </si>
-  <si>
     <t xml:space="preserve">CHIES</t>
   </si>
   <si>
     <t xml:space="preserve">frequenza luoghi di culto</t>
   </si>
   <si>
-    <t xml:space="preserve">spiritualità</t>
+    <t xml:space="preserve">spirituality</t>
   </si>
   <si>
     <t xml:space="preserve">SITEC</t>
@@ -673,7 +751,10 @@
     <t xml:space="preserve">soddisfazione situa economica ultimi 12 mesi</t>
   </si>
   <si>
-    <t xml:space="preserve">livello di soddisfazione</t>
+    <t xml:space="preserve">satisfaction_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QOL_aggr</t>
   </si>
   <si>
     <t xml:space="preserve">SALUT</t>
@@ -718,15 +799,15 @@
     <t xml:space="preserve">selezionare solo persone che lavorano</t>
   </si>
   <si>
+    <t xml:space="preserve">Nas are for CONDMi=1 (occupato). Substitute these Nas with 0=not working</t>
+  </si>
+  <si>
     <t xml:space="preserve">PPAPO      </t>
   </si>
   <si>
     <t xml:space="preserve">partecipato ultimi 12 mesi a riunioni di partiti politici</t>
   </si>
   <si>
-    <t xml:space="preserve">vita sociale – strutturata</t>
-  </si>
-  <si>
     <t xml:space="preserve">SOC_LIFE_STRUTT_aggr</t>
   </si>
   <si>
@@ -760,6 +841,12 @@
     <t xml:space="preserve">partecipato ultimi 12 mesi a riunioni di associazioni professionali-categoria</t>
   </si>
   <si>
+    <t xml:space="preserve">VOLON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">svolto volontariato per associazioni ultimi 12 mesi</t>
+  </si>
+  <si>
     <t xml:space="preserve">INCSPI</t>
   </si>
   <si>
@@ -770,6 +857,12 @@
   </si>
   <si>
     <t xml:space="preserve">indice massa corporea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mental health (ricostruita dalle var sf)</t>
   </si>
   <si>
     <t xml:space="preserve">RISEC</t>
@@ -990,22 +1083,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A84" activeCellId="0" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="54.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="50.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="54.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="48.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="30"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="45.97"/>
@@ -1030,19 +1122,31 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,10 +1154,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,13 +1165,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,16 +1179,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1092,10 +1196,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,13 +1207,16 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1117,13 +1224,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,19 +1238,16 @@
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,13 +1255,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,13 +1272,25 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,19 +1298,28 @@
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>24</v>
+      <c r="I12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,13 +1327,16 @@
         <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1213,13 +1344,19 @@
         <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1227,13 +1364,19 @@
         <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1241,13 +1384,19 @@
         <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,13 +1404,19 @@
         <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1269,13 +1424,31 @@
         <v>67</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1283,19 +1456,31 @@
         <v>69</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1303,19 +1488,31 @@
         <v>71</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J20" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1323,1469 +1520,1651 @@
         <v>73</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>50</v>
+        <v>71</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>50</v>
+        <v>71</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>48</v>
+      <c r="I24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>71</v>
+        <v>102</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
-        <v>128</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>78</v>
+        <v>130</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>130</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>84</v>
+        <v>132</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F43" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F44" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>109</v>
+        <v>136</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>80</v>
+        <v>138</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>80</v>
+        <v>138</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>116</v>
+        <v>144</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J49" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>116</v>
+        <v>144</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J50" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>120</v>
+        <v>151</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>121</v>
+        <v>138</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J52" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
-        <v>158</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>124</v>
+        <v>161</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>115</v>
+        <v>138</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="D54" s="1" t="s">
-        <v>115</v>
+        <v>138</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="D55" s="1" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="C56" s="1" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>116</v>
+        <v>138</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J56" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>116</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>134</v>
+        <v>169</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>121</v>
+        <v>168</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J58" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>115</v>
+        <v>168</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J59" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>138</v>
+        <v>176</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>140</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>141</v>
+        <v>179</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>142</v>
+        <v>180</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>140</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>143</v>
+        <v>181</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>140</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>48</v>
+        <v>184</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>48</v>
+        <v>188</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>48</v>
+        <v>191</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>151</v>
+        <v>193</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>152</v>
+        <v>194</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>153</v>
+        <v>185</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>155</v>
+        <v>195</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>156</v>
+        <v>196</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>153</v>
+        <v>185</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="D68" s="3" t="s">
-        <v>153</v>
+        <v>45</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>160</v>
+        <v>29</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I68" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J68" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>161</v>
+        <v>201</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>162</v>
+        <v>202</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>153</v>
+        <v>45</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>157</v>
+        <v>29</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>153</v>
+        <v>45</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>154</v>
+        <v>29</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
-        <v>202</v>
+        <v>227</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>165</v>
+        <v>207</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>166</v>
+        <v>208</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E71" s="1" t="n">
-        <v>99</v>
+        <v>45</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>24</v>
+        <v>209</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>169</v>
+        <v>211</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E72" s="1" t="n">
-        <v>99</v>
+        <v>45</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>24</v>
+        <v>209</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
-        <v>207</v>
+        <v>229</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>170</v>
+        <v>212</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>171</v>
+        <v>213</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>167</v>
+        <v>45</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F74" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>176</v>
+        <v>216</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>177</v>
+        <v>217</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>174</v>
+        <v>45</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>178</v>
+        <v>218</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>179</v>
+        <v>219</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>174</v>
+        <v>45</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>181</v>
+        <v>221</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>174</v>
+        <v>45</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>183</v>
+        <v>223</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>174</v>
+        <v>45</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
-        <v>231</v>
+        <v>341</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>184</v>
+        <v>224</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>185</v>
+        <v>225</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
-        <v>232</v>
+        <v>342</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>187</v>
+        <v>228</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
+        <v>344</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H81" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>175</v>
+      <c r="I81" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="n">
+        <v>345</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="C82" s="1" t="s">
-        <v>191</v>
+        <v>235</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>175</v>
+        <v>231</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I82" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="n">
+        <v>346</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="C83" s="1" t="s">
-        <v>193</v>
+        <v>237</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I83" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="C84" s="1" t="s">
-        <v>195</v>
+        <v>239</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="n">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>196</v>
+        <v>241</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>197</v>
+        <v>242</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>199</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="n">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>200</v>
+        <v>245</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>201</v>
+        <v>246</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>199</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="n">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>202</v>
+        <v>247</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>203</v>
+        <v>248</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>204</v>
+        <v>243</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="n">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>206</v>
+        <v>249</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>207</v>
+        <v>250</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>204</v>
+        <v>243</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>205</v>
+        <v>244</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="n">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>208</v>
+        <v>251</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>209</v>
+        <v>252</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>204</v>
+        <v>243</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>205</v>
+        <v>244</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="n">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>210</v>
+        <v>254</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>211</v>
+        <v>255</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>167</v>
+        <v>243</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>212</v>
+        <v>256</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>213</v>
+        <v>257</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>214</v>
+        <v>243</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I91" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J91" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="n">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>215</v>
+        <v>260</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>217</v>
+        <v>93</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="n">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>219</v>
+        <v>263</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>264</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>217</v>
+        <v>93</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="n">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>221</v>
+        <v>265</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>266</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>217</v>
+        <v>93</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="n">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>223</v>
+        <v>267</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>268</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>217</v>
+        <v>93</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="n">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>225</v>
+        <v>269</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>270</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>226</v>
+        <v>93</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="n">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>228</v>
+        <v>271</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>217</v>
+        <v>93</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="n">
-        <v>358</v>
+        <v>371</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>230</v>
+        <v>273</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>274</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>217</v>
+        <v>93</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>226</v>
+        <v>46</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="n">
-        <v>360</v>
+        <v>375</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>233</v>
+        <v>275</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>276</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="n">
-        <v>361</v>
+        <v>526</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>237</v>
+        <v>277</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>235</v>
+        <v>61</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="n">
-        <v>362</v>
+      <c r="A101" s="3" t="n">
+        <v>527</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>239</v>
+        <v>279</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>235</v>
+        <v>185</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="n">
-        <v>363</v>
+        <v>708</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>241</v>
+        <v>281</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>282</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="1" t="n">
-        <v>364</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C103" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="1" t="n">
-        <v>365</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="n">
-        <v>375</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="1" t="n">
-        <v>526</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="1" t="n">
-        <v>708</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>